<commit_message>
fix: mise a jour du template excel 2
</commit_message>
<xml_diff>
--- a/server/static/mission-locale/modele-rupturant-ml.xlsx
+++ b/server/static/mission-locale/modele-rupturant-ml.xlsx
@@ -3,13 +3,13 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28715"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2AA5ED26-2CAB-48AD-8CD4-7BF724F4D7C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{1B8A3A6E-B8A0-4737-92E5-F4E92D7D142D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="2" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Lisez-moi" sheetId="1" r:id="rId1"/>
-    <sheet name="à traiter (nouveaux)" sheetId="2" r:id="rId2"/>
+    <sheet name="à traiter" sheetId="2" r:id="rId2"/>
     <sheet name="déjà traités" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191028" iterateDelta="1E-4"/>
@@ -467,7 +467,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A74C061-002F-43CC-8B84-A3D6ECD81113}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
@@ -484,8 +484,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDBAB42B-161C-418B-9208-60D10F584D0D}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
-      <selection sqref="A1:W1048576"/>
+    <sheetView topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="L23" sqref="L23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>

</xml_diff>

<commit_message>
fix: mise a jour du template excel 3
</commit_message>
<xml_diff>
--- a/server/static/mission-locale/modele-rupturant-ml.xlsx
+++ b/server/static/mission-locale/modele-rupturant-ml.xlsx
@@ -3,14 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28715"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1B8A3A6E-B8A0-4737-92E5-F4E92D7D142D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{9A79B171-CF12-4BD0-80D5-08C8E9F10B03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="2" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Lisez-moi" sheetId="1" r:id="rId1"/>
-    <sheet name="à traiter" sheetId="2" r:id="rId2"/>
-    <sheet name="déjà traités" sheetId="3" r:id="rId3"/>
+    <sheet name="À traiter" sheetId="2" r:id="rId2"/>
+    <sheet name="Déjà traités" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191028" iterateDelta="1E-4"/>
   <extLst>
@@ -467,7 +467,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A74C061-002F-43CC-8B84-A3D6ECD81113}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
@@ -484,7 +484,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDBAB42B-161C-418B-9208-60D10F584D0D}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView topLeftCell="K1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
       <selection activeCell="L23" sqref="L23"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
fix: mise a jour du template excel 3 (#4142)
</commit_message>
<xml_diff>
--- a/server/static/mission-locale/modele-rupturant-ml.xlsx
+++ b/server/static/mission-locale/modele-rupturant-ml.xlsx
@@ -3,14 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28715"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1B8A3A6E-B8A0-4737-92E5-F4E92D7D142D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{9A79B171-CF12-4BD0-80D5-08C8E9F10B03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="2" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Lisez-moi" sheetId="1" r:id="rId1"/>
-    <sheet name="à traiter" sheetId="2" r:id="rId2"/>
-    <sheet name="déjà traités" sheetId="3" r:id="rId3"/>
+    <sheet name="À traiter" sheetId="2" r:id="rId2"/>
+    <sheet name="Déjà traités" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191028" iterateDelta="1E-4"/>
   <extLst>
@@ -467,7 +467,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A74C061-002F-43CC-8B84-A3D6ECD81113}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
@@ -484,7 +484,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDBAB42B-161C-418B-9208-60D10F584D0D}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView topLeftCell="K1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
       <selection activeCell="L23" sqref="L23"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
fix: mise a jour du fichier d'export ml
</commit_message>
<xml_diff>
--- a/server/static/mission-locale/modele-rupturant-ml.xlsx
+++ b/server/static/mission-locale/modele-rupturant-ml.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28715"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28724"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9A79B171-CF12-4BD0-80D5-08C8E9F10B03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{DB5D7A9C-A57B-47F9-9FC9-EBF481176AC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="2" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Lisez-moi" sheetId="1" r:id="rId1"/>
@@ -467,13 +467,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A74C061-002F-43CC-8B84-A3D6ECD81113}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+    <sheetView tabSelected="1" topLeftCell="AJ1" workbookViewId="0">
+      <selection activeCell="X1" sqref="X1:AX1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="23" width="15.7109375" customWidth="1"/>
+    <col min="1" max="50" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -484,8 +484,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDBAB42B-161C-418B-9208-60D10F584D0D}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="L23" sqref="L23"/>
+    <sheetView topLeftCell="AX1" workbookViewId="0">
+      <selection activeCell="X1" sqref="X1:BI1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>

</xml_diff>

<commit_message>
fix: mise a jour du fichier d'export ml (#4157)
</commit_message>
<xml_diff>
--- a/server/static/mission-locale/modele-rupturant-ml.xlsx
+++ b/server/static/mission-locale/modele-rupturant-ml.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28715"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28724"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9A79B171-CF12-4BD0-80D5-08C8E9F10B03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{DB5D7A9C-A57B-47F9-9FC9-EBF481176AC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="2" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Lisez-moi" sheetId="1" r:id="rId1"/>
@@ -467,13 +467,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A74C061-002F-43CC-8B84-A3D6ECD81113}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+    <sheetView tabSelected="1" topLeftCell="AJ1" workbookViewId="0">
+      <selection activeCell="X1" sqref="X1:AX1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="23" width="15.7109375" customWidth="1"/>
+    <col min="1" max="50" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -484,8 +484,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDBAB42B-161C-418B-9208-60D10F584D0D}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="L23" sqref="L23"/>
+    <sheetView topLeftCell="AX1" workbookViewId="0">
+      <selection activeCell="X1" sqref="X1:BI1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>

</xml_diff>

<commit_message>
feat: ajout des onglets sur l'export des missions locales
</commit_message>
<xml_diff>
--- a/server/static/mission-locale/modele-rupturant-ml.xlsx
+++ b/server/static/mission-locale/modele-rupturant-ml.xlsx
@@ -1,16 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28724"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28830"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DB5D7A9C-A57B-47F9-9FC9-EBF481176AC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{331EEE3A-0CCE-4976-BE02-1FF3E26A6454}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="2" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Lisez-moi" sheetId="1" r:id="rId1"/>
     <sheet name="À traiter" sheetId="2" r:id="rId2"/>
     <sheet name="Déjà traités" sheetId="3" r:id="rId3"/>
+    <sheet name="Injoignable" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191028" iterateDelta="1E-4"/>
   <extLst>
@@ -467,8 +468,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A74C061-002F-43CC-8B84-A3D6ECD81113}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AJ1" workbookViewId="0">
-      <selection activeCell="X1" sqref="X1:AX1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="X1" sqref="X1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -484,8 +485,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDBAB42B-161C-418B-9208-60D10F584D0D}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView topLeftCell="AX1" workbookViewId="0">
-      <selection activeCell="X1" sqref="X1:BI1048576"/>
+    <sheetView topLeftCell="P12" workbookViewId="0">
+      <selection activeCell="T21" sqref="T21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -495,4 +496,21 @@
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20662541-ED35-46C9-9BE9-18373F74D06E}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="AK1" workbookViewId="0">
+      <selection sqref="A1:CF1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75"/>
+  <cols>
+    <col min="1" max="84" width="15.7109375" customWidth="1"/>
+  </cols>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
feat: ajout des onglets sur l'export des missions locales (#4213)
</commit_message>
<xml_diff>
--- a/server/static/mission-locale/modele-rupturant-ml.xlsx
+++ b/server/static/mission-locale/modele-rupturant-ml.xlsx
@@ -1,16 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28724"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28830"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DB5D7A9C-A57B-47F9-9FC9-EBF481176AC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{331EEE3A-0CCE-4976-BE02-1FF3E26A6454}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="2" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Lisez-moi" sheetId="1" r:id="rId1"/>
     <sheet name="À traiter" sheetId="2" r:id="rId2"/>
     <sheet name="Déjà traités" sheetId="3" r:id="rId3"/>
+    <sheet name="Injoignable" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191028" iterateDelta="1E-4"/>
   <extLst>
@@ -467,8 +468,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A74C061-002F-43CC-8B84-A3D6ECD81113}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AJ1" workbookViewId="0">
-      <selection activeCell="X1" sqref="X1:AX1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="X1" sqref="X1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -484,8 +485,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDBAB42B-161C-418B-9208-60D10F584D0D}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView topLeftCell="AX1" workbookViewId="0">
-      <selection activeCell="X1" sqref="X1:BI1048576"/>
+    <sheetView topLeftCell="P12" workbookViewId="0">
+      <selection activeCell="T21" sqref="T21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -495,4 +496,21 @@
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20662541-ED35-46C9-9BE9-18373F74D06E}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="AK1" workbookViewId="0">
+      <selection sqref="A1:CF1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75"/>
+  <cols>
+    <col min="1" max="84" width="15.7109375" customWidth="1"/>
+  </cols>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
fix: correction d'erreur sur l'ouverture du fichier excel
</commit_message>
<xml_diff>
--- a/server/static/mission-locale/modele-rupturant-ml.xlsx
+++ b/server/static/mission-locale/modele-rupturant-ml.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28908"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{331EEE3A-0CCE-4976-BE02-1FF3E26A6454}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{14349CC4-8499-4835-A449-C57844EF4148}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="3" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Lisez-moi" sheetId="1" r:id="rId1"/>
@@ -468,7 +468,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A74C061-002F-43CC-8B84-A3D6ECD81113}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="P1" workbookViewId="0">
       <selection activeCell="X1" sqref="X1"/>
     </sheetView>
   </sheetViews>
@@ -485,13 +485,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDBAB42B-161C-418B-9208-60D10F584D0D}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView topLeftCell="P12" workbookViewId="0">
-      <selection activeCell="T21" sqref="T21"/>
+    <sheetView tabSelected="1" topLeftCell="O12" workbookViewId="0">
+      <selection activeCell="X1" sqref="X1:AF1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="23" width="15.7109375" customWidth="1"/>
+    <col min="1" max="32" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -502,9 +502,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20662541-ED35-46C9-9BE9-18373F74D06E}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AK1" workbookViewId="0">
-      <selection sqref="A1:CF1048576"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>

</xml_diff>

<commit_message>
fix: correction d'erreur sur l'ouverture du fichier excel (#4224)
</commit_message>
<xml_diff>
--- a/server/static/mission-locale/modele-rupturant-ml.xlsx
+++ b/server/static/mission-locale/modele-rupturant-ml.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28908"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{331EEE3A-0CCE-4976-BE02-1FF3E26A6454}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{14349CC4-8499-4835-A449-C57844EF4148}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="3" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Lisez-moi" sheetId="1" r:id="rId1"/>
@@ -468,7 +468,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A74C061-002F-43CC-8B84-A3D6ECD81113}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="P1" workbookViewId="0">
       <selection activeCell="X1" sqref="X1"/>
     </sheetView>
   </sheetViews>
@@ -485,13 +485,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDBAB42B-161C-418B-9208-60D10F584D0D}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView topLeftCell="P12" workbookViewId="0">
-      <selection activeCell="T21" sqref="T21"/>
+    <sheetView tabSelected="1" topLeftCell="O12" workbookViewId="0">
+      <selection activeCell="X1" sqref="X1:AF1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="23" width="15.7109375" customWidth="1"/>
+    <col min="1" max="32" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -502,9 +502,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20662541-ED35-46C9-9BE9-18373F74D06E}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AK1" workbookViewId="0">
-      <selection sqref="A1:CF1048576"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>

</xml_diff>